<commit_message>
add MultiFilterFixed and TokenAttrFilter, modified the SpecialFilter to not yield duplicates
</commit_message>
<xml_diff>
--- a/recordcleaner/Web_ADV_Report_CBOT.xlsx
+++ b/recordcleaner/Web_ADV_Report_CBOT.xlsx
@@ -6,7 +6,7 @@
     <s:workbookView activeTab="0"/>
   </s:bookViews>
   <s:sheets>
-    <s:sheet name="ADV 28-02-2018" sheetId="1" r:id="rId1"/>
+    <s:sheet name="ADV 29-03-2018" sheetId="1" r:id="rId1"/>
   </s:sheets>
   <s:definedNames/>
   <s:calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -19,18 +19,18 @@
     <t>Product</t>
   </si>
   <si>
+    <t>ADV MAR 2018</t>
+  </si>
+  <si>
+    <t>ADV MAR 2017</t>
+  </si>
+  <si>
+    <t>% CHG</t>
+  </si>
+  <si>
     <t>ADV FEB 2018</t>
   </si>
   <si>
-    <t>ADV FEB 2017</t>
-  </si>
-  <si>
-    <t>% CHG</t>
-  </si>
-  <si>
-    <t>ADV JAN 2018</t>
-  </si>
-  <si>
     <t>ADV Y.T.D 2018</t>
   </si>
   <si>
@@ -82,6 +82,9 @@
     <t>Options</t>
   </si>
   <si>
+    <t>-</t>
+  </si>
+  <si>
     <t>DJ US REAL ESTATE</t>
   </si>
   <si>
@@ -146,9 +149,6 @@
   </si>
   <si>
     <t>SOYBEAN CRUSH</t>
-  </si>
-  <si>
-    <t>-</t>
   </si>
   <si>
     <t>JULY-DEC CORN CAL SPRD</t>
@@ -570,7 +570,7 @@
     <col customWidth="1" max="1" min="1" width="29"/>
     <col customWidth="1" max="2" min="2" width="14"/>
     <col customWidth="1" max="3" min="3" width="14"/>
-    <col customWidth="1" max="4" min="4" width="8"/>
+    <col customWidth="1" max="4" min="4" width="9"/>
     <col customWidth="1" max="5" min="5" width="14"/>
     <col customWidth="1" max="6" min="6" width="8"/>
     <col customWidth="1" max="7" min="7" width="16"/>
@@ -620,28 +620,28 @@
         <v>9</v>
       </c>
       <c r="B2" t="n">
-        <v>556522</v>
+        <v>303807</v>
       </c>
       <c r="C2" t="n">
-        <v>376296.58</v>
+        <v>252966.3</v>
       </c>
       <c r="D2" t="n">
-        <v>47.9</v>
+        <v>20.1</v>
       </c>
       <c r="E2" t="n">
-        <v>316591.05</v>
+        <v>556521.53</v>
       </c>
       <c r="F2" t="n">
-        <v>75.8</v>
+        <v>-45.4</v>
       </c>
       <c r="G2" t="n">
-        <v>430558</v>
+        <v>386922</v>
       </c>
       <c r="H2" t="n">
-        <v>315782</v>
+        <v>292479</v>
       </c>
       <c r="I2" t="n">
-        <v>36.3</v>
+        <v>32.3</v>
       </c>
       <c r="J2" t="s">
         <v>10</v>
@@ -655,28 +655,28 @@
         <v>12</v>
       </c>
       <c r="B3" t="n">
-        <v>2713445</v>
+        <v>1611292</v>
       </c>
       <c r="C3" t="n">
-        <v>2032587</v>
+        <v>1287341.91</v>
       </c>
       <c r="D3" t="n">
-        <v>33.5</v>
+        <v>25.2</v>
       </c>
       <c r="E3" t="n">
-        <v>1568530.76</v>
+        <v>2713444.74</v>
       </c>
       <c r="F3" t="n">
-        <v>73</v>
+        <v>-40.6</v>
       </c>
       <c r="G3" t="n">
-        <v>2112365</v>
+        <v>1939864</v>
       </c>
       <c r="H3" t="n">
-        <v>1722349</v>
+        <v>1560975</v>
       </c>
       <c r="I3" t="n">
-        <v>22.6</v>
+        <v>24.3</v>
       </c>
       <c r="J3" t="s">
         <v>10</v>
@@ -690,28 +690,28 @@
         <v>13</v>
       </c>
       <c r="B4" t="n">
-        <v>1862560</v>
+        <v>951173</v>
       </c>
       <c r="C4" t="n">
-        <v>1420569.53</v>
+        <v>761297.87</v>
       </c>
       <c r="D4" t="n">
-        <v>31.1</v>
+        <v>24.9</v>
       </c>
       <c r="E4" t="n">
-        <v>871543.24</v>
+        <v>1862559.63</v>
       </c>
       <c r="F4" t="n">
-        <v>113.7</v>
+        <v>-48.9</v>
       </c>
       <c r="G4" t="n">
-        <v>1342276</v>
+        <v>1207634</v>
       </c>
       <c r="H4" t="n">
-        <v>1092679</v>
+        <v>969747</v>
       </c>
       <c r="I4" t="n">
-        <v>22.8</v>
+        <v>24.5</v>
       </c>
       <c r="J4" t="s">
         <v>10</v>
@@ -725,28 +725,28 @@
         <v>14</v>
       </c>
       <c r="B5" t="n">
-        <v>1018381</v>
+        <v>459631</v>
       </c>
       <c r="C5" t="n">
-        <v>571075.16</v>
+        <v>299720.39</v>
       </c>
       <c r="D5" t="n">
-        <v>78.3</v>
+        <v>53.4</v>
       </c>
       <c r="E5" t="n">
-        <v>391763.71</v>
+        <v>1018380.74</v>
       </c>
       <c r="F5" t="n">
-        <v>159.9</v>
+        <v>-54.9</v>
       </c>
       <c r="G5" t="n">
-        <v>689407</v>
+        <v>610304</v>
       </c>
       <c r="H5" t="n">
-        <v>425729</v>
+        <v>378984</v>
       </c>
       <c r="I5" t="n">
-        <v>61.9</v>
+        <v>61</v>
       </c>
       <c r="J5" t="s">
         <v>10</v>
@@ -760,28 +760,28 @@
         <v>15</v>
       </c>
       <c r="B6" t="n">
-        <v>371279</v>
+        <v>290824</v>
       </c>
       <c r="C6" t="n">
-        <v>334010.37</v>
+        <v>260551.39</v>
       </c>
       <c r="D6" t="n">
-        <v>11.2</v>
+        <v>11.6</v>
       </c>
       <c r="E6" t="n">
-        <v>195572.33</v>
+        <v>371278.74</v>
       </c>
       <c r="F6" t="n">
-        <v>89.8</v>
+        <v>-21.7</v>
       </c>
       <c r="G6" t="n">
-        <v>279033</v>
+        <v>283092</v>
       </c>
       <c r="H6" t="n">
-        <v>246590</v>
+        <v>251769</v>
       </c>
       <c r="I6" t="n">
-        <v>13.2</v>
+        <v>12.4</v>
       </c>
       <c r="J6" t="s">
         <v>10</v>
@@ -795,28 +795,28 @@
         <v>16</v>
       </c>
       <c r="B7" t="n">
-        <v>947</v>
+        <v>2721</v>
       </c>
       <c r="C7" t="n">
-        <v>2470.16</v>
+        <v>3649.3</v>
       </c>
       <c r="D7" t="n">
-        <v>-61.7</v>
+        <v>-25.4</v>
       </c>
       <c r="E7" t="n">
-        <v>1335.19</v>
+        <v>946.58</v>
       </c>
       <c r="F7" t="n">
-        <v>-29.1</v>
+        <v>187.5</v>
       </c>
       <c r="G7" t="n">
-        <v>1151</v>
+        <v>1691</v>
       </c>
       <c r="H7" t="n">
-        <v>2775</v>
+        <v>3099</v>
       </c>
       <c r="I7" t="n">
-        <v>-58.5</v>
+        <v>-45.4</v>
       </c>
       <c r="J7" t="s">
         <v>10</v>
@@ -830,28 +830,28 @@
         <v>17</v>
       </c>
       <c r="B8" t="n">
-        <v>2391</v>
+        <v>4727</v>
       </c>
       <c r="C8" t="n">
-        <v>1993.37</v>
+        <v>4198.52</v>
       </c>
       <c r="D8" t="n">
-        <v>19.9</v>
+        <v>12.6</v>
       </c>
       <c r="E8" t="n">
-        <v>1668.62</v>
+        <v>2390.84</v>
       </c>
       <c r="F8" t="n">
-        <v>43.3</v>
+        <v>97.7</v>
       </c>
       <c r="G8" t="n">
-        <v>2012</v>
+        <v>2946</v>
       </c>
       <c r="H8" t="n">
-        <v>1846</v>
+        <v>2719</v>
       </c>
       <c r="I8" t="n">
-        <v>9</v>
+        <v>8.4</v>
       </c>
       <c r="J8" t="s">
         <v>10</v>
@@ -865,28 +865,28 @@
         <v>18</v>
       </c>
       <c r="B9" t="n">
-        <v>318049</v>
+        <v>132627</v>
       </c>
       <c r="C9" t="n">
-        <v>200607.05</v>
+        <v>100353.96</v>
       </c>
       <c r="D9" t="n">
-        <v>58.5</v>
+        <v>32.2</v>
       </c>
       <c r="E9" t="n">
-        <v>130208.81</v>
+        <v>318049.05</v>
       </c>
       <c r="F9" t="n">
-        <v>144.3</v>
+        <v>-58.3</v>
       </c>
       <c r="G9" t="n">
-        <v>219433</v>
+        <v>189549</v>
       </c>
       <c r="H9" t="n">
-        <v>148431</v>
+        <v>130596</v>
       </c>
       <c r="I9" t="n">
-        <v>47.8</v>
+        <v>45.1</v>
       </c>
       <c r="J9" t="s">
         <v>10</v>
@@ -900,28 +900,28 @@
         <v>19</v>
       </c>
       <c r="B10" t="n">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C10" t="n">
-        <v>49.11</v>
+        <v>116.87</v>
       </c>
       <c r="D10" t="n">
-        <v>-82</v>
+        <v>-87.09999999999999</v>
       </c>
       <c r="E10" t="n">
-        <v>16.19</v>
+        <v>8.84</v>
       </c>
       <c r="F10" t="n">
-        <v>-45.4</v>
+        <v>70.7</v>
       </c>
       <c r="G10" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H10" t="n">
-        <v>61</v>
+        <v>82</v>
       </c>
       <c r="I10" t="n">
-        <v>-79.3</v>
+        <v>-83.5</v>
       </c>
       <c r="J10" t="s">
         <v>10</v>
@@ -935,28 +935,28 @@
         <v>20</v>
       </c>
       <c r="B11" t="n">
-        <v>310180</v>
+        <v>168251</v>
       </c>
       <c r="C11" t="n">
-        <v>137039.32</v>
+        <v>79854</v>
       </c>
       <c r="D11" t="n">
-        <v>126.3</v>
+        <v>110.7</v>
       </c>
       <c r="E11" t="n">
-        <v>150570.86</v>
+        <v>310179.53</v>
       </c>
       <c r="F11" t="n">
-        <v>106</v>
+        <v>-45.8</v>
       </c>
       <c r="G11" t="n">
-        <v>226385</v>
+        <v>206371</v>
       </c>
       <c r="H11" t="n">
-        <v>117561</v>
+        <v>103573</v>
       </c>
       <c r="I11" t="n">
-        <v>92.59999999999999</v>
+        <v>99.3</v>
       </c>
       <c r="J11" t="s">
         <v>10</v>
@@ -970,28 +970,28 @@
         <v>9</v>
       </c>
       <c r="B12" t="n">
-        <v>180930</v>
+        <v>108762</v>
       </c>
       <c r="C12" t="n">
-        <v>102371.16</v>
+        <v>94813.22</v>
       </c>
       <c r="D12" t="n">
-        <v>76.7</v>
+        <v>14.7</v>
       </c>
       <c r="E12" t="n">
-        <v>142944.05</v>
+        <v>180929.84</v>
       </c>
       <c r="F12" t="n">
-        <v>26.6</v>
+        <v>-39.9</v>
       </c>
       <c r="G12" t="n">
-        <v>160987</v>
+        <v>143008</v>
       </c>
       <c r="H12" t="n">
-        <v>97167</v>
+        <v>96294</v>
       </c>
       <c r="I12" t="n">
-        <v>65.7</v>
+        <v>48.5</v>
       </c>
       <c r="J12" t="s">
         <v>10</v>
@@ -1005,28 +1005,28 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>917331</v>
+        <v>622639</v>
       </c>
       <c r="C13" t="n">
-        <v>508993.68</v>
+        <v>487277.39</v>
       </c>
       <c r="D13" t="n">
-        <v>80.2</v>
+        <v>27.8</v>
       </c>
       <c r="E13" t="n">
-        <v>633564.05</v>
+        <v>917331.11</v>
       </c>
       <c r="F13" t="n">
-        <v>44.8</v>
+        <v>-32.1</v>
       </c>
       <c r="G13" t="n">
-        <v>768353</v>
+        <v>718189</v>
       </c>
       <c r="H13" t="n">
-        <v>523196</v>
+        <v>509872</v>
       </c>
       <c r="I13" t="n">
-        <v>46.9</v>
+        <v>40.9</v>
       </c>
       <c r="J13" t="s">
         <v>10</v>
@@ -1040,28 +1040,28 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>255572</v>
+        <v>159679</v>
       </c>
       <c r="C14" t="n">
-        <v>143200.74</v>
+        <v>167507.61</v>
       </c>
       <c r="D14" t="n">
-        <v>78.5</v>
+        <v>-4.7</v>
       </c>
       <c r="E14" t="n">
-        <v>152076.29</v>
+        <v>255572.26</v>
       </c>
       <c r="F14" t="n">
-        <v>68.09999999999999</v>
+        <v>-37.5</v>
       </c>
       <c r="G14" t="n">
-        <v>201237</v>
+        <v>186930</v>
       </c>
       <c r="H14" t="n">
-        <v>133752</v>
+        <v>146274</v>
       </c>
       <c r="I14" t="n">
-        <v>50.5</v>
+        <v>27.8</v>
       </c>
       <c r="J14" t="s">
         <v>10</v>
@@ -1075,28 +1075,28 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>32390</v>
+        <v>21153</v>
       </c>
       <c r="C15" t="n">
-        <v>6090.16</v>
+        <v>5147.3</v>
       </c>
       <c r="D15" t="n">
-        <v>431.8</v>
+        <v>311</v>
       </c>
       <c r="E15" t="n">
-        <v>14590</v>
+        <v>32390.32</v>
       </c>
       <c r="F15" t="n">
-        <v>122</v>
+        <v>-34.7</v>
       </c>
       <c r="G15" t="n">
-        <v>23045</v>
+        <v>22394</v>
       </c>
       <c r="H15" t="n">
-        <v>4368</v>
+        <v>4657</v>
       </c>
       <c r="I15" t="n">
-        <v>427.6</v>
+        <v>380.9</v>
       </c>
       <c r="J15" t="s">
         <v>10</v>
@@ -1110,28 +1110,28 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>147</v>
+        <v>287</v>
       </c>
       <c r="C16" t="n">
-        <v>125.05</v>
+        <v>70.78</v>
       </c>
       <c r="D16" t="n">
-        <v>17.3</v>
+        <v>305.7</v>
       </c>
       <c r="E16" t="n">
-        <v>35.76</v>
+        <v>146.63</v>
       </c>
       <c r="F16" t="n">
-        <v>310</v>
+        <v>95.8</v>
       </c>
       <c r="G16" t="n">
-        <v>88</v>
+        <v>157</v>
       </c>
       <c r="H16" t="n">
-        <v>176</v>
+        <v>137</v>
       </c>
       <c r="I16" t="n">
-        <v>-49.8</v>
+        <v>14.3</v>
       </c>
       <c r="J16" t="s">
         <v>10</v>
@@ -1145,28 +1145,28 @@
         <v>18</v>
       </c>
       <c r="B17" t="n">
+        <v>243</v>
+      </c>
+      <c r="C17" t="n">
+        <v>82.17</v>
+      </c>
+      <c r="D17" t="n">
+        <v>195.3</v>
+      </c>
+      <c r="E17" t="n">
         <v>247</v>
       </c>
-      <c r="C17" t="n">
-        <v>57.63</v>
-      </c>
-      <c r="D17" t="n">
-        <v>328.6</v>
-      </c>
-      <c r="E17" t="n">
-        <v>176.71</v>
-      </c>
       <c r="F17" t="n">
-        <v>39.8</v>
+        <v>-1.8</v>
       </c>
       <c r="G17" t="n">
-        <v>210</v>
+        <v>221</v>
       </c>
       <c r="H17" t="n">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I17" t="n">
-        <v>162.5</v>
+        <v>173.8</v>
       </c>
       <c r="J17" t="s">
         <v>10</v>
@@ -1183,25 +1183,25 @@
         <v>0</v>
       </c>
       <c r="C18" t="n">
-        <v>56.74</v>
+        <v>232.52</v>
       </c>
       <c r="D18" t="n">
-        <v>-100</v>
+        <v>-99.90000000000001</v>
       </c>
       <c r="E18" t="n">
-        <v>1.19</v>
-      </c>
-      <c r="F18" t="n">
-        <v>-100</v>
+        <v>0</v>
+      </c>
+      <c r="F18" t="s">
+        <v>22</v>
       </c>
       <c r="G18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H18" t="n">
-        <v>39</v>
+        <v>111</v>
       </c>
       <c r="I18" t="n">
-        <v>-98.40000000000001</v>
+        <v>-99.59999999999999</v>
       </c>
       <c r="J18" t="s">
         <v>10</v>
@@ -1212,34 +1212,34 @@
     </row>
     <row r="19" spans="1:11">
       <c r="A19" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B19" t="n">
-        <v>2543</v>
+        <v>3385</v>
       </c>
       <c r="C19" t="n">
-        <v>582</v>
+        <v>2180.7</v>
       </c>
       <c r="D19" t="n">
-        <v>336.9</v>
+        <v>55.2</v>
       </c>
       <c r="E19" t="n">
-        <v>1407.1</v>
+        <v>2542.63</v>
       </c>
       <c r="F19" t="n">
-        <v>80.7</v>
+        <v>33.1</v>
       </c>
       <c r="G19" t="n">
-        <v>1946</v>
+        <v>2442</v>
       </c>
       <c r="H19" t="n">
-        <v>742</v>
+        <v>1276</v>
       </c>
       <c r="I19" t="n">
-        <v>162.3</v>
+        <v>91.40000000000001</v>
       </c>
       <c r="J19" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="K19" t="s">
         <v>11</v>
@@ -1247,34 +1247,34 @@
     </row>
     <row r="20" spans="1:11">
       <c r="A20" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" t="n">
+        <v>330467</v>
+      </c>
+      <c r="C20" t="n">
+        <v>169213.96</v>
+      </c>
+      <c r="D20" t="n">
+        <v>95.3</v>
+      </c>
+      <c r="E20" t="n">
+        <v>346951.95</v>
+      </c>
+      <c r="F20" t="n">
+        <v>-4.8</v>
+      </c>
+      <c r="G20" t="n">
+        <v>281232</v>
+      </c>
+      <c r="H20" t="n">
+        <v>141147</v>
+      </c>
+      <c r="I20" t="n">
+        <v>99.2</v>
+      </c>
+      <c r="J20" t="s">
         <v>24</v>
-      </c>
-      <c r="B20" t="n">
-        <v>346952</v>
-      </c>
-      <c r="C20" t="n">
-        <v>123346</v>
-      </c>
-      <c r="D20" t="n">
-        <v>181.3</v>
-      </c>
-      <c r="E20" t="n">
-        <v>172536.48</v>
-      </c>
-      <c r="F20" t="n">
-        <v>101.1</v>
-      </c>
-      <c r="G20" t="n">
-        <v>255384</v>
-      </c>
-      <c r="H20" t="n">
-        <v>124595</v>
-      </c>
-      <c r="I20" t="n">
-        <v>105</v>
-      </c>
-      <c r="J20" t="s">
-        <v>23</v>
       </c>
       <c r="K20" t="s">
         <v>11</v>
@@ -1282,34 +1282,34 @@
     </row>
     <row r="21" spans="1:11">
       <c r="A21" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" t="n">
+        <v>674</v>
+      </c>
+      <c r="C21" t="n">
+        <v>296.57</v>
+      </c>
+      <c r="D21" t="n">
+        <v>127.3</v>
+      </c>
+      <c r="E21" t="n">
+        <v>806.26</v>
+      </c>
+      <c r="F21" t="n">
+        <v>-16.4</v>
+      </c>
+      <c r="G21" t="n">
+        <v>647</v>
+      </c>
+      <c r="H21" t="n">
+        <v>301</v>
+      </c>
+      <c r="I21" t="n">
+        <v>114.8</v>
+      </c>
+      <c r="J21" t="s">
         <v>24</v>
-      </c>
-      <c r="B21" t="n">
-        <v>806</v>
-      </c>
-      <c r="C21" t="n">
-        <v>292.11</v>
-      </c>
-      <c r="D21" t="n">
-        <v>176</v>
-      </c>
-      <c r="E21" t="n">
-        <v>474.43</v>
-      </c>
-      <c r="F21" t="n">
-        <v>69.90000000000001</v>
-      </c>
-      <c r="G21" t="n">
-        <v>632</v>
-      </c>
-      <c r="H21" t="n">
-        <v>304</v>
-      </c>
-      <c r="I21" t="n">
-        <v>108.1</v>
-      </c>
-      <c r="J21" t="s">
-        <v>23</v>
       </c>
       <c r="K21" t="s">
         <v>21</v>
@@ -1317,34 +1317,34 @@
     </row>
     <row r="22" spans="1:11">
       <c r="A22" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B22" t="n">
-        <v>485</v>
+        <v>413</v>
       </c>
       <c r="C22" t="n">
-        <v>822.63</v>
+        <v>809</v>
       </c>
       <c r="D22" t="n">
-        <v>-41.1</v>
+        <v>-48.9</v>
       </c>
       <c r="E22" t="n">
-        <v>500.1</v>
+        <v>484.89</v>
       </c>
       <c r="F22" t="n">
-        <v>-3</v>
+        <v>-14.7</v>
       </c>
       <c r="G22" t="n">
-        <v>493</v>
+        <v>466</v>
       </c>
       <c r="H22" t="n">
-        <v>885</v>
+        <v>857</v>
       </c>
       <c r="I22" t="n">
-        <v>-44.3</v>
+        <v>-45.7</v>
       </c>
       <c r="J22" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="K22" t="s">
         <v>11</v>
@@ -1352,34 +1352,34 @@
     </row>
     <row r="23" spans="1:11">
       <c r="A23" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B23" t="n">
-        <v>569410</v>
+        <v>416886</v>
       </c>
       <c r="C23" t="n">
-        <v>441013.89</v>
+        <v>260945.87</v>
       </c>
       <c r="D23" t="n">
-        <v>29.1</v>
+        <v>59.8</v>
       </c>
       <c r="E23" t="n">
-        <v>308311.48</v>
+        <v>569410.47</v>
       </c>
       <c r="F23" t="n">
-        <v>84.7</v>
+        <v>-26.8</v>
       </c>
       <c r="G23" t="n">
-        <v>432334</v>
+        <v>427016</v>
       </c>
       <c r="H23" t="n">
-        <v>366423</v>
+        <v>327294</v>
       </c>
       <c r="I23" t="n">
-        <v>18</v>
+        <v>30.5</v>
       </c>
       <c r="J23" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K23" t="s">
         <v>11</v>
@@ -1387,34 +1387,34 @@
     </row>
     <row r="24" spans="1:11">
       <c r="A24" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B24" t="n">
-        <v>357869</v>
+        <v>243629</v>
       </c>
       <c r="C24" t="n">
-        <v>273532.16</v>
+        <v>166825.39</v>
       </c>
       <c r="D24" t="n">
-        <v>30.8</v>
+        <v>46</v>
       </c>
       <c r="E24" t="n">
-        <v>193662.29</v>
+        <v>357868.53</v>
       </c>
       <c r="F24" t="n">
-        <v>84.8</v>
+        <v>-31.9</v>
       </c>
       <c r="G24" t="n">
-        <v>271660</v>
+        <v>262010</v>
       </c>
       <c r="H24" t="n">
-        <v>229687</v>
+        <v>206368</v>
       </c>
       <c r="I24" t="n">
-        <v>18.3</v>
+        <v>27</v>
       </c>
       <c r="J24" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K24" t="s">
         <v>11</v>
@@ -1422,34 +1422,34 @@
     </row>
     <row r="25" spans="1:11">
       <c r="A25" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B25" t="n">
-        <v>182469</v>
+        <v>109283</v>
       </c>
       <c r="C25" t="n">
-        <v>113534.37</v>
+        <v>80625.87</v>
       </c>
       <c r="D25" t="n">
-        <v>60.7</v>
+        <v>35.5</v>
       </c>
       <c r="E25" t="n">
-        <v>118210.62</v>
+        <v>182469.32</v>
       </c>
       <c r="F25" t="n">
-        <v>54.4</v>
+        <v>-40.1</v>
       </c>
       <c r="G25" t="n">
-        <v>148734</v>
+        <v>135152</v>
       </c>
       <c r="H25" t="n">
-        <v>102965</v>
+        <v>94678</v>
       </c>
       <c r="I25" t="n">
-        <v>44.4</v>
+        <v>42.7</v>
       </c>
       <c r="J25" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K25" t="s">
         <v>11</v>
@@ -1457,34 +1457,34 @@
     </row>
     <row r="26" spans="1:11">
       <c r="A26" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B26" t="n">
-        <v>184373</v>
+        <v>104061</v>
       </c>
       <c r="C26" t="n">
-        <v>144081.68</v>
+        <v>105288.48</v>
       </c>
       <c r="D26" t="n">
-        <v>28</v>
+        <v>-1.2</v>
       </c>
       <c r="E26" t="n">
-        <v>101297.52</v>
+        <v>184373.16</v>
       </c>
       <c r="F26" t="n">
-        <v>82</v>
+        <v>-43.6</v>
       </c>
       <c r="G26" t="n">
-        <v>140758</v>
+        <v>128125</v>
       </c>
       <c r="H26" t="n">
-        <v>121517</v>
+        <v>115497</v>
       </c>
       <c r="I26" t="n">
-        <v>15.8</v>
+        <v>10.9</v>
       </c>
       <c r="J26" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K26" t="s">
         <v>11</v>
@@ -1492,34 +1492,34 @@
     </row>
     <row r="27" spans="1:11">
       <c r="A27" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B27" t="n">
-        <v>785</v>
+        <v>701</v>
       </c>
       <c r="C27" t="n">
-        <v>878.47</v>
+        <v>573.04</v>
       </c>
       <c r="D27" t="n">
+        <v>22.3</v>
+      </c>
+      <c r="E27" t="n">
+        <v>784.89</v>
+      </c>
+      <c r="F27" t="n">
         <v>-10.7</v>
       </c>
-      <c r="E27" t="n">
-        <v>744.4299999999999</v>
-      </c>
-      <c r="F27" t="n">
-        <v>5.4</v>
-      </c>
       <c r="G27" t="n">
-        <v>764</v>
+        <v>742</v>
       </c>
       <c r="H27" t="n">
-        <v>816</v>
+        <v>726</v>
       </c>
       <c r="I27" t="n">
-        <v>-6.4</v>
+        <v>2.2</v>
       </c>
       <c r="J27" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K27" t="s">
         <v>11</v>
@@ -1527,34 +1527,34 @@
     </row>
     <row r="28" spans="1:11">
       <c r="A28" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B28" t="n">
-        <v>1177</v>
+        <v>422</v>
       </c>
       <c r="C28" t="n">
-        <v>1988.47</v>
+        <v>531.48</v>
       </c>
       <c r="D28" t="n">
-        <v>-40.8</v>
+        <v>-20.6</v>
       </c>
       <c r="E28" t="n">
-        <v>799.1</v>
+        <v>1177.21</v>
       </c>
       <c r="F28" t="n">
-        <v>47.3</v>
+        <v>-64.09999999999999</v>
       </c>
       <c r="G28" t="n">
-        <v>979</v>
+        <v>787</v>
       </c>
       <c r="H28" t="n">
-        <v>1279</v>
+        <v>1002</v>
       </c>
       <c r="I28" t="n">
-        <v>-23.5</v>
+        <v>-21.4</v>
       </c>
       <c r="J28" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K28" t="s">
         <v>11</v>
@@ -1562,34 +1562,34 @@
     </row>
     <row r="29" spans="1:11">
       <c r="A29" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B29" t="n">
-        <v>300</v>
+        <v>525</v>
       </c>
       <c r="C29" t="n">
-        <v>371.84</v>
+        <v>443.43</v>
       </c>
       <c r="D29" t="n">
-        <v>-19.3</v>
+        <v>18.4</v>
       </c>
       <c r="E29" t="n">
-        <v>177.62</v>
+        <v>300.11</v>
       </c>
       <c r="F29" t="n">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="G29" t="n">
-        <v>236</v>
+        <v>335</v>
       </c>
       <c r="H29" t="n">
-        <v>531</v>
+        <v>499</v>
       </c>
       <c r="I29" t="n">
-        <v>-55.6</v>
+        <v>-32.7</v>
       </c>
       <c r="J29" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K29" t="s">
         <v>11</v>
@@ -1597,34 +1597,34 @@
     </row>
     <row r="30" spans="1:11">
       <c r="A30" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B30" t="n">
+        <v>569</v>
+      </c>
+      <c r="C30" t="n">
+        <v>317.13</v>
+      </c>
+      <c r="D30" t="n">
+        <v>79.40000000000001</v>
+      </c>
+      <c r="E30" t="n">
         <v>551</v>
       </c>
-      <c r="C30" t="n">
-        <v>564.16</v>
-      </c>
-      <c r="D30" t="n">
-        <v>-2.3</v>
-      </c>
-      <c r="E30" t="n">
-        <v>395.29</v>
-      </c>
       <c r="F30" t="n">
-        <v>39.4</v>
+        <v>3.2</v>
       </c>
       <c r="G30" t="n">
-        <v>469</v>
+        <v>504</v>
       </c>
       <c r="H30" t="n">
-        <v>486</v>
+        <v>423</v>
       </c>
       <c r="I30" t="n">
-        <v>-3.4</v>
+        <v>19</v>
       </c>
       <c r="J30" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K30" t="s">
         <v>11</v>
@@ -1632,34 +1632,34 @@
     </row>
     <row r="31" spans="1:11">
       <c r="A31" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B31" t="n">
-        <v>2014</v>
+        <v>1585</v>
       </c>
       <c r="C31" t="n">
-        <v>1080.11</v>
+        <v>618</v>
       </c>
       <c r="D31" t="n">
-        <v>86.5</v>
+        <v>156.5</v>
       </c>
       <c r="E31" t="n">
-        <v>1019.24</v>
+        <v>2014.32</v>
       </c>
       <c r="F31" t="n">
-        <v>97.59999999999999</v>
+        <v>-21.3</v>
       </c>
       <c r="G31" t="n">
-        <v>1492</v>
+        <v>1524</v>
       </c>
       <c r="H31" t="n">
-        <v>1070</v>
+        <v>903</v>
       </c>
       <c r="I31" t="n">
-        <v>39.4</v>
+        <v>68.8</v>
       </c>
       <c r="J31" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K31" t="s">
         <v>11</v>
@@ -1667,34 +1667,34 @@
     </row>
     <row r="32" spans="1:11">
       <c r="A32" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B32" t="n">
-        <v>337</v>
+        <v>347</v>
       </c>
       <c r="C32" t="n">
-        <v>352.47</v>
+        <v>181.7</v>
       </c>
       <c r="D32" t="n">
-        <v>-4.3</v>
+        <v>90.8</v>
       </c>
       <c r="E32" t="n">
-        <v>205.29</v>
+        <v>337.26</v>
       </c>
       <c r="F32" t="n">
-        <v>64.3</v>
+        <v>2.8</v>
       </c>
       <c r="G32" t="n">
-        <v>268</v>
+        <v>295</v>
       </c>
       <c r="H32" t="n">
-        <v>307</v>
+        <v>261</v>
       </c>
       <c r="I32" t="n">
-        <v>-12.8</v>
+        <v>13.2</v>
       </c>
       <c r="J32" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K32" t="s">
         <v>11</v>
@@ -1702,34 +1702,34 @@
     </row>
     <row r="33" spans="1:11">
       <c r="A33" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B33" t="n">
-        <v>3008</v>
+        <v>6350</v>
       </c>
       <c r="C33" t="n">
-        <v>860.6799999999999</v>
+        <v>5935</v>
       </c>
       <c r="D33" t="n">
-        <v>249.5</v>
+        <v>7</v>
       </c>
       <c r="E33" t="n">
-        <v>3633.62</v>
+        <v>3007.79</v>
       </c>
       <c r="F33" t="n">
-        <v>-17.2</v>
+        <v>111.1</v>
       </c>
       <c r="G33" t="n">
-        <v>3336</v>
+        <v>4374</v>
       </c>
       <c r="H33" t="n">
-        <v>926</v>
+        <v>2784</v>
       </c>
       <c r="I33" t="n">
-        <v>260.3</v>
+        <v>57.1</v>
       </c>
       <c r="J33" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K33" t="s">
         <v>11</v>
@@ -1737,34 +1737,34 @@
     </row>
     <row r="34" spans="1:11">
       <c r="A34" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B34" t="n">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="C34" t="n">
-        <v>73.42</v>
+        <v>72.39</v>
       </c>
       <c r="D34" t="n">
-        <v>71.7</v>
+        <v>61.5</v>
       </c>
       <c r="E34" t="n">
-        <v>70.23999999999999</v>
+        <v>126.05</v>
       </c>
       <c r="F34" t="n">
-        <v>79.5</v>
+        <v>-7.3</v>
       </c>
       <c r="G34" t="n">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="H34" t="n">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="I34" t="n">
-        <v>25.1</v>
+        <v>37.4</v>
       </c>
       <c r="J34" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K34" t="s">
         <v>11</v>
@@ -1772,34 +1772,34 @@
     </row>
     <row r="35" spans="1:11">
       <c r="A35" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B35" t="n">
-        <v>4</v>
+        <v>78</v>
       </c>
       <c r="C35" t="n">
-        <v>8.630000000000001</v>
+        <v>93.04000000000001</v>
       </c>
       <c r="D35" t="n">
-        <v>-50</v>
+        <v>-15.8</v>
       </c>
       <c r="E35" t="n">
-        <v>31.24</v>
+        <v>4.32</v>
       </c>
       <c r="F35" t="n">
-        <v>-86.2</v>
+        <v>1716.1</v>
       </c>
       <c r="G35" t="n">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="H35" t="n">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="I35" t="n">
-        <v>46.2</v>
+        <v>-7.9</v>
       </c>
       <c r="J35" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K35" t="s">
         <v>11</v>
@@ -1807,34 +1807,34 @@
     </row>
     <row r="36" spans="1:11">
       <c r="A36" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B36" t="n">
+        <v>145015</v>
+      </c>
+      <c r="C36" t="n">
+        <v>99736.03999999999</v>
+      </c>
+      <c r="D36" t="n">
+        <v>45.4</v>
+      </c>
+      <c r="E36" t="n">
         <v>196380</v>
       </c>
-      <c r="C36" t="n">
-        <v>167943</v>
-      </c>
-      <c r="D36" t="n">
-        <v>16.9</v>
-      </c>
-      <c r="E36" t="n">
-        <v>128558.48</v>
-      </c>
       <c r="F36" t="n">
-        <v>52.8</v>
+        <v>-26.2</v>
       </c>
       <c r="G36" t="n">
-        <v>160774</v>
+        <v>155349</v>
       </c>
       <c r="H36" t="n">
-        <v>142960</v>
+        <v>126925</v>
       </c>
       <c r="I36" t="n">
-        <v>12.5</v>
+        <v>22.4</v>
       </c>
       <c r="J36" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K36" t="s">
         <v>11</v>
@@ -1842,34 +1842,34 @@
     </row>
     <row r="37" spans="1:11">
       <c r="A37" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B37" t="n">
+        <v>64807</v>
+      </c>
+      <c r="C37" t="n">
+        <v>36192.04</v>
+      </c>
+      <c r="D37" t="n">
+        <v>79.09999999999999</v>
+      </c>
+      <c r="E37" t="n">
         <v>98659</v>
       </c>
-      <c r="C37" t="n">
-        <v>55588.58</v>
-      </c>
-      <c r="D37" t="n">
-        <v>77.5</v>
-      </c>
-      <c r="E37" t="n">
-        <v>61742.81</v>
-      </c>
       <c r="F37" t="n">
-        <v>59.8</v>
+        <v>-34.3</v>
       </c>
       <c r="G37" t="n">
-        <v>79278</v>
+        <v>74296</v>
       </c>
       <c r="H37" t="n">
-        <v>48930</v>
+        <v>44205</v>
       </c>
       <c r="I37" t="n">
-        <v>62</v>
+        <v>68.09999999999999</v>
       </c>
       <c r="J37" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K37" t="s">
         <v>11</v>
@@ -1877,34 +1877,34 @@
     </row>
     <row r="38" spans="1:11">
       <c r="A38" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B38" t="n">
-        <v>76143</v>
+        <v>120535</v>
       </c>
       <c r="C38" t="n">
-        <v>96539.95</v>
+        <v>89289.74000000001</v>
       </c>
       <c r="D38" t="n">
-        <v>-21.1</v>
+        <v>35</v>
       </c>
       <c r="E38" t="n">
-        <v>79590.52</v>
+        <v>76142.67999999999</v>
       </c>
       <c r="F38" t="n">
-        <v>-4.3</v>
+        <v>58.3</v>
       </c>
       <c r="G38" t="n">
-        <v>77953</v>
+        <v>92612</v>
       </c>
       <c r="H38" t="n">
-        <v>82800</v>
+        <v>85207</v>
       </c>
       <c r="I38" t="n">
-        <v>-5.9</v>
+        <v>8.699999999999999</v>
       </c>
       <c r="J38" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K38" t="s">
         <v>21</v>
@@ -1912,34 +1912,34 @@
     </row>
     <row r="39" spans="1:11">
       <c r="A39" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B39" t="n">
-        <v>97096</v>
+        <v>85772</v>
       </c>
       <c r="C39" t="n">
-        <v>61097.37</v>
+        <v>68811</v>
       </c>
       <c r="D39" t="n">
-        <v>58.9</v>
+        <v>24.6</v>
       </c>
       <c r="E39" t="n">
-        <v>64723.57</v>
+        <v>97096.05</v>
       </c>
       <c r="F39" t="n">
-        <v>50</v>
+        <v>-11.7</v>
       </c>
       <c r="G39" t="n">
-        <v>80101</v>
+        <v>82053</v>
       </c>
       <c r="H39" t="n">
-        <v>60736</v>
+        <v>63731</v>
       </c>
       <c r="I39" t="n">
-        <v>31.9</v>
+        <v>28.7</v>
       </c>
       <c r="J39" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K39" t="s">
         <v>21</v>
@@ -1947,34 +1947,34 @@
     </row>
     <row r="40" spans="1:11">
       <c r="A40" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B40" t="n">
-        <v>21381</v>
+        <v>16927</v>
       </c>
       <c r="C40" t="n">
-        <v>7589</v>
+        <v>9173.83</v>
       </c>
       <c r="D40" t="n">
-        <v>181.7</v>
+        <v>84.5</v>
       </c>
       <c r="E40" t="n">
-        <v>12923.48</v>
+        <v>21380.58</v>
       </c>
       <c r="F40" t="n">
-        <v>65.40000000000001</v>
+        <v>-20.8</v>
       </c>
       <c r="G40" t="n">
-        <v>16941</v>
+        <v>16936</v>
       </c>
       <c r="H40" t="n">
-        <v>8662</v>
+        <v>8852</v>
       </c>
       <c r="I40" t="n">
-        <v>95.59999999999999</v>
+        <v>91.3</v>
       </c>
       <c r="J40" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K40" t="s">
         <v>21</v>
@@ -1982,34 +1982,34 @@
     </row>
     <row r="41" spans="1:11">
       <c r="A41" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B41" t="n">
-        <v>7131</v>
+        <v>6775</v>
       </c>
       <c r="C41" t="n">
-        <v>8168.21</v>
+        <v>10163.09</v>
       </c>
       <c r="D41" t="n">
-        <v>-12.7</v>
+        <v>-33.3</v>
       </c>
       <c r="E41" t="n">
-        <v>5733.81</v>
+        <v>7131.16</v>
       </c>
       <c r="F41" t="n">
-        <v>24.4</v>
+        <v>-5</v>
       </c>
       <c r="G41" t="n">
-        <v>6398</v>
+        <v>6528</v>
       </c>
       <c r="H41" t="n">
-        <v>7641</v>
+        <v>8577</v>
       </c>
       <c r="I41" t="n">
-        <v>-16.3</v>
+        <v>-23.9</v>
       </c>
       <c r="J41" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K41" t="s">
         <v>21</v>
@@ -2017,22 +2017,22 @@
     </row>
     <row r="42" spans="1:11">
       <c r="A42" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B42" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C42" t="n">
-        <v>0.26</v>
+        <v>3.7</v>
       </c>
       <c r="D42" t="n">
-        <v>519.9</v>
+        <v>-60.1</v>
       </c>
       <c r="E42" t="n">
-        <v>0.48</v>
+        <v>1.63</v>
       </c>
       <c r="F42" t="n">
-        <v>242.6</v>
+        <v>-9.5</v>
       </c>
       <c r="G42" t="n">
         <v>1</v>
@@ -2041,10 +2041,10 @@
         <v>3</v>
       </c>
       <c r="I42" t="n">
-        <v>-61.9</v>
+        <v>-61.5</v>
       </c>
       <c r="J42" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K42" t="s">
         <v>21</v>
@@ -2052,34 +2052,34 @@
     </row>
     <row r="43" spans="1:11">
       <c r="A43" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B43" t="n">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="C43" t="n">
-        <v>50.26</v>
+        <v>49.26</v>
       </c>
       <c r="D43" t="n">
-        <v>-59.8</v>
+        <v>-32.7</v>
       </c>
       <c r="E43" t="n">
-        <v>21.38</v>
+        <v>20.21</v>
       </c>
       <c r="F43" t="n">
-        <v>-5.5</v>
+        <v>64</v>
       </c>
       <c r="G43" t="n">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="H43" t="n">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="I43" t="n">
-        <v>-68.3</v>
+        <v>-57.9</v>
       </c>
       <c r="J43" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K43" t="s">
         <v>21</v>
@@ -2087,34 +2087,34 @@
     </row>
     <row r="44" spans="1:11">
       <c r="A44" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B44" t="n">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="C44" t="n">
-        <v>62.16</v>
+        <v>36.43</v>
       </c>
       <c r="D44" t="n">
-        <v>-15.7</v>
+        <v>4</v>
       </c>
       <c r="E44" t="n">
-        <v>102.05</v>
+        <v>52.37</v>
       </c>
       <c r="F44" t="n">
-        <v>-48.7</v>
+        <v>-27.6</v>
       </c>
       <c r="G44" t="n">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="H44" t="n">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="I44" t="n">
         <v>12.3</v>
       </c>
       <c r="J44" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K44" t="s">
         <v>21</v>
@@ -2122,34 +2122,34 @@
     </row>
     <row r="45" spans="1:11">
       <c r="A45" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B45" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C45" t="n">
-        <v>0</v>
-      </c>
-      <c r="D45" t="s">
-        <v>44</v>
+        <v>3.17</v>
+      </c>
+      <c r="D45" t="n">
+        <v>50</v>
       </c>
       <c r="E45" t="n">
-        <v>16.05</v>
+        <v>6.68</v>
       </c>
       <c r="F45" t="n">
-        <v>-58.3</v>
+        <v>-28.8</v>
       </c>
       <c r="G45" t="n">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H45" t="n">
-        <v>0</v>
-      </c>
-      <c r="I45" t="s">
-        <v>44</v>
+        <v>1</v>
+      </c>
+      <c r="I45" t="n">
+        <v>685.3</v>
       </c>
       <c r="J45" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K45" t="s">
         <v>21</v>
@@ -2160,31 +2160,31 @@
         <v>45</v>
       </c>
       <c r="B46" t="n">
-        <v>17</v>
+        <v>200</v>
       </c>
       <c r="C46" t="n">
-        <v>31.58</v>
+        <v>104.35</v>
       </c>
       <c r="D46" t="n">
-        <v>-47.5</v>
+        <v>91.7</v>
       </c>
       <c r="E46" t="n">
-        <v>4.95</v>
+        <v>16.58</v>
       </c>
       <c r="F46" t="n">
-        <v>234.8</v>
+        <v>1106.3</v>
       </c>
       <c r="G46" t="n">
-        <v>10</v>
+        <v>76</v>
       </c>
       <c r="H46" t="n">
-        <v>23</v>
+        <v>53</v>
       </c>
       <c r="I46" t="n">
-        <v>-54.6</v>
+        <v>42.3</v>
       </c>
       <c r="J46" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K46" t="s">
         <v>21</v>
@@ -2195,31 +2195,31 @@
         <v>46</v>
       </c>
       <c r="B47" t="n">
-        <v>708</v>
+        <v>926</v>
       </c>
       <c r="C47" t="n">
-        <v>532.53</v>
+        <v>845.83</v>
       </c>
       <c r="D47" t="n">
-        <v>32.9</v>
+        <v>9.5</v>
       </c>
       <c r="E47" t="n">
-        <v>146.33</v>
+        <v>707.89</v>
       </c>
       <c r="F47" t="n">
-        <v>383.8</v>
+        <v>30.8</v>
       </c>
       <c r="G47" t="n">
-        <v>413</v>
+        <v>590</v>
       </c>
       <c r="H47" t="n">
-        <v>601</v>
+        <v>692</v>
       </c>
       <c r="I47" t="n">
-        <v>-31.2</v>
+        <v>-14.7</v>
       </c>
       <c r="J47" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K47" t="s">
         <v>21</v>
@@ -2233,7 +2233,7 @@
         <v>0</v>
       </c>
       <c r="C48" t="n">
-        <v>11.05</v>
+        <v>4.35</v>
       </c>
       <c r="D48" t="n">
         <v>-100</v>
@@ -2242,19 +2242,19 @@
         <v>0</v>
       </c>
       <c r="F48" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="G48" t="n">
         <v>0</v>
       </c>
       <c r="H48" t="n">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="I48" t="n">
         <v>-100</v>
       </c>
       <c r="J48" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K48" t="s">
         <v>21</v>
@@ -2265,31 +2265,31 @@
         <v>48</v>
       </c>
       <c r="B49" t="n">
-        <v>239</v>
+        <v>44</v>
       </c>
       <c r="C49" t="n">
-        <v>86.73999999999999</v>
+        <v>40.78</v>
       </c>
       <c r="D49" t="n">
-        <v>175.2</v>
+        <v>8.6</v>
       </c>
       <c r="E49" t="n">
-        <v>47.14</v>
+        <v>238.74</v>
       </c>
       <c r="F49" t="n">
-        <v>406.4</v>
+        <v>-81.40000000000001</v>
       </c>
       <c r="G49" t="n">
-        <v>138</v>
+        <v>106</v>
       </c>
       <c r="H49" t="n">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="I49" t="n">
-        <v>91.5</v>
+        <v>74.90000000000001</v>
       </c>
       <c r="J49" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K49" t="s">
         <v>21</v>
@@ -2300,31 +2300,31 @@
         <v>49</v>
       </c>
       <c r="B50" t="n">
+        <v>136</v>
+      </c>
+      <c r="C50" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="D50" t="n">
+        <v>31091.1</v>
+      </c>
+      <c r="E50" t="n">
         <v>100</v>
       </c>
-      <c r="C50" t="n">
-        <v>51.58</v>
-      </c>
-      <c r="D50" t="n">
-        <v>93.90000000000001</v>
-      </c>
-      <c r="E50" t="n">
-        <v>92.86</v>
-      </c>
       <c r="F50" t="n">
-        <v>7.7</v>
+        <v>35.6</v>
       </c>
       <c r="G50" t="n">
-        <v>96</v>
+        <v>110</v>
       </c>
       <c r="H50" t="n">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="I50" t="n">
-        <v>55.1</v>
+        <v>180.2</v>
       </c>
       <c r="J50" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K50" t="s">
         <v>21</v>
@@ -2341,13 +2341,13 @@
         <v>0</v>
       </c>
       <c r="D51" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="E51" t="n">
         <v>0</v>
       </c>
       <c r="F51" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="G51" t="n">
         <v>0</v>
@@ -2356,10 +2356,10 @@
         <v>0</v>
       </c>
       <c r="I51" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="J51" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K51" t="s">
         <v>21</v>
@@ -2376,25 +2376,25 @@
         <v>0</v>
       </c>
       <c r="D52" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="E52" t="n">
-        <v>0.43</v>
-      </c>
-      <c r="F52" t="n">
-        <v>-100</v>
+        <v>0</v>
+      </c>
+      <c r="F52" t="s">
+        <v>22</v>
       </c>
       <c r="G52" t="n">
         <v>0</v>
       </c>
       <c r="H52" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I52" t="n">
-        <v>-86.3</v>
+        <v>-85.7</v>
       </c>
       <c r="J52" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K52" t="s">
         <v>21</v>
@@ -2405,31 +2405,31 @@
         <v>52</v>
       </c>
       <c r="B53" t="n">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C53" t="n">
-        <v>0</v>
-      </c>
-      <c r="D53" t="s">
-        <v>44</v>
+        <v>34.78</v>
+      </c>
+      <c r="D53" t="n">
+        <v>-69.2</v>
       </c>
       <c r="E53" t="n">
-        <v>0</v>
-      </c>
-      <c r="F53" t="s">
-        <v>44</v>
+        <v>13.16</v>
+      </c>
+      <c r="F53" t="n">
+        <v>-18.6</v>
       </c>
       <c r="G53" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H53" t="n">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="I53" t="n">
-        <v>-30.4</v>
+        <v>-58</v>
       </c>
       <c r="J53" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K53" t="s">
         <v>21</v>
@@ -2443,28 +2443,28 @@
         <v>0</v>
       </c>
       <c r="C54" t="n">
-        <v>0</v>
-      </c>
-      <c r="D54" t="s">
-        <v>44</v>
+        <v>143.48</v>
+      </c>
+      <c r="D54" t="n">
+        <v>-100</v>
       </c>
       <c r="E54" t="n">
         <v>0</v>
       </c>
       <c r="F54" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="G54" t="n">
         <v>0</v>
       </c>
       <c r="H54" t="n">
-        <v>15</v>
+        <v>63</v>
       </c>
       <c r="I54" t="n">
         <v>-100</v>
       </c>
       <c r="J54" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K54" t="s">
         <v>21</v>
@@ -2475,31 +2475,31 @@
         <v>54</v>
       </c>
       <c r="B55" t="n">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="C55" t="n">
-        <v>0.53</v>
+        <v>1.61</v>
       </c>
       <c r="D55" t="n">
-        <v>2910.1</v>
+        <v>2131.9</v>
       </c>
       <c r="E55" t="n">
-        <v>1</v>
+        <v>15.84</v>
       </c>
       <c r="F55" t="n">
-        <v>1484.2</v>
+        <v>126.6</v>
       </c>
       <c r="G55" t="n">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="H55" t="n">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="I55" t="n">
-        <v>-72.8</v>
+        <v>-8.1</v>
       </c>
       <c r="J55" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K55" t="s">
         <v>21</v>
@@ -2513,16 +2513,16 @@
         <v>0</v>
       </c>
       <c r="C56" t="n">
-        <v>0</v>
-      </c>
-      <c r="D56" t="s">
-        <v>44</v>
+        <v>1.09</v>
+      </c>
+      <c r="D56" t="n">
+        <v>-100</v>
       </c>
       <c r="E56" t="n">
-        <v>0.05</v>
-      </c>
-      <c r="F56" t="n">
-        <v>-100</v>
+        <v>0</v>
+      </c>
+      <c r="F56" t="s">
+        <v>22</v>
       </c>
       <c r="G56" t="n">
         <v>0</v>
@@ -2530,11 +2530,11 @@
       <c r="H56" t="n">
         <v>0</v>
       </c>
-      <c r="I56" t="s">
-        <v>44</v>
+      <c r="I56" t="n">
+        <v>-95.90000000000001</v>
       </c>
       <c r="J56" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K56" t="s">
         <v>21</v>
@@ -2548,7 +2548,7 @@
         <v>0</v>
       </c>
       <c r="C57" t="n">
-        <v>5</v>
+        <v>4.35</v>
       </c>
       <c r="D57" t="n">
         <v>-100</v>
@@ -2557,19 +2557,19 @@
         <v>0</v>
       </c>
       <c r="F57" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="G57" t="n">
         <v>0</v>
       </c>
       <c r="H57" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I57" t="n">
         <v>-100</v>
       </c>
       <c r="J57" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K57" t="s">
         <v>21</v>
@@ -2580,31 +2580,31 @@
         <v>57</v>
       </c>
       <c r="B58" t="n">
-        <v>71</v>
+        <v>0</v>
       </c>
       <c r="C58" t="n">
-        <v>92.31999999999999</v>
-      </c>
-      <c r="D58" t="n">
-        <v>-22.7</v>
+        <v>0</v>
+      </c>
+      <c r="D58" t="s">
+        <v>22</v>
       </c>
       <c r="E58" t="n">
-        <v>32.86</v>
+        <v>71.31999999999999</v>
       </c>
       <c r="F58" t="n">
-        <v>117</v>
+        <v>-100</v>
       </c>
       <c r="G58" t="n">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="H58" t="n">
-        <v>63</v>
+        <v>40</v>
       </c>
       <c r="I58" t="n">
-        <v>-18.7</v>
+        <v>-15.2</v>
       </c>
       <c r="J58" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K58" t="s">
         <v>21</v>
@@ -2621,13 +2621,13 @@
         <v>0</v>
       </c>
       <c r="D59" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="E59" t="n">
         <v>0</v>
       </c>
       <c r="F59" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="G59" t="n">
         <v>0</v>
@@ -2636,10 +2636,10 @@
         <v>0</v>
       </c>
       <c r="I59" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="J59" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K59" t="s">
         <v>21</v>
@@ -2653,28 +2653,28 @@
         <v>0</v>
       </c>
       <c r="C60" t="n">
-        <v>30.11</v>
-      </c>
-      <c r="D60" t="n">
-        <v>-100</v>
+        <v>0</v>
+      </c>
+      <c r="D60" t="s">
+        <v>22</v>
       </c>
       <c r="E60" t="n">
-        <v>9.52</v>
-      </c>
-      <c r="F60" t="n">
-        <v>-100</v>
+        <v>0</v>
+      </c>
+      <c r="F60" t="s">
+        <v>22</v>
       </c>
       <c r="G60" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H60" t="n">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="I60" t="n">
-        <v>-85.8</v>
+        <v>-85.2</v>
       </c>
       <c r="J60" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K60" t="s">
         <v>21</v>
@@ -2682,34 +2682,34 @@
     </row>
     <row r="61" spans="1:11">
       <c r="A61" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B61" t="n">
-        <v>36225</v>
+        <v>40014</v>
       </c>
       <c r="C61" t="n">
-        <v>32818.58</v>
+        <v>27358.74</v>
       </c>
       <c r="D61" t="n">
-        <v>10.4</v>
+        <v>46.3</v>
       </c>
       <c r="E61" t="n">
-        <v>41729.43</v>
+        <v>36224.74</v>
       </c>
       <c r="F61" t="n">
-        <v>-13.2</v>
+        <v>10.5</v>
       </c>
       <c r="G61" t="n">
-        <v>39115</v>
+        <v>39424</v>
       </c>
       <c r="H61" t="n">
-        <v>30731</v>
+        <v>29480</v>
       </c>
       <c r="I61" t="n">
-        <v>27.3</v>
+        <v>33.7</v>
       </c>
       <c r="J61" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K61" t="s">
         <v>21</v>
@@ -2726,13 +2726,13 @@
         <v>0</v>
       </c>
       <c r="D62" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="E62" t="n">
         <v>0</v>
       </c>
       <c r="F62" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="G62" t="n">
         <v>0</v>
@@ -2741,10 +2741,10 @@
         <v>0</v>
       </c>
       <c r="I62" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="J62" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K62" t="s">
         <v>21</v>
@@ -2761,13 +2761,13 @@
         <v>0</v>
       </c>
       <c r="D63" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="E63" t="n">
         <v>0</v>
       </c>
       <c r="F63" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="G63" t="n">
         <v>0</v>
@@ -2776,10 +2776,10 @@
         <v>0</v>
       </c>
       <c r="I63" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="J63" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K63" t="s">
         <v>21</v>
@@ -2790,31 +2790,31 @@
         <v>62</v>
       </c>
       <c r="B64" t="n">
-        <v>84</v>
+        <v>32</v>
       </c>
       <c r="C64" t="n">
-        <v>5.26</v>
-      </c>
-      <c r="D64" t="n">
-        <v>1498</v>
+        <v>0</v>
+      </c>
+      <c r="D64" t="s">
+        <v>22</v>
       </c>
       <c r="E64" t="n">
-        <v>234.76</v>
+        <v>84.11</v>
       </c>
       <c r="F64" t="n">
-        <v>-64.2</v>
+        <v>-62</v>
       </c>
       <c r="G64" t="n">
-        <v>163</v>
+        <v>118</v>
       </c>
       <c r="H64" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I64" t="n">
-        <v>3066.6</v>
+        <v>3540.9</v>
       </c>
       <c r="J64" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K64" t="s">
         <v>21</v>
@@ -2822,34 +2822,34 @@
     </row>
     <row r="65" spans="1:11">
       <c r="A65" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B65" t="n">
-        <v>4895</v>
+        <v>5760</v>
       </c>
       <c r="C65" t="n">
-        <v>1640.26</v>
+        <v>1667.91</v>
       </c>
       <c r="D65" t="n">
-        <v>198.5</v>
+        <v>245.4</v>
       </c>
       <c r="E65" t="n">
-        <v>4089.43</v>
+        <v>4895.42</v>
       </c>
       <c r="F65" t="n">
-        <v>19.7</v>
+        <v>17.7</v>
       </c>
       <c r="G65" t="n">
-        <v>4472</v>
+        <v>4916</v>
       </c>
       <c r="H65" t="n">
-        <v>1601</v>
+        <v>1626</v>
       </c>
       <c r="I65" t="n">
-        <v>179.3</v>
+        <v>202.3</v>
       </c>
       <c r="J65" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K65" t="s">
         <v>21</v>
@@ -2857,31 +2857,31 @@
     </row>
     <row r="66" spans="1:11">
       <c r="A66" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B66" t="n">
-        <v>51</v>
+        <v>21</v>
       </c>
       <c r="C66" t="n">
         <v>0</v>
       </c>
       <c r="D66" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="E66" t="n">
-        <v>107.14</v>
+        <v>51.32</v>
       </c>
       <c r="F66" t="n">
-        <v>-52.1</v>
+        <v>-58.2</v>
       </c>
       <c r="G66" t="n">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="H66" t="n">
         <v>0</v>
       </c>
       <c r="I66" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="J66" t="s">
         <v>63</v>

</xml_diff>